<commit_message>
Atualizando o andamento das SARs.
</commit_message>
<xml_diff>
--- a/Artefatos de Documentação/Processo Aplicado/EveRemind/1-Gerencia de Requisitos/Histórico de SARs.xlsx
+++ b/Artefatos de Documentação/Processo Aplicado/EveRemind/1-Gerencia de Requisitos/Histórico de SARs.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
   <si>
     <t>SAR ID</t>
   </si>
@@ -41,12 +41,6 @@
     <t>BAIXA</t>
   </si>
   <si>
-    <t>Encerrada</t>
-  </si>
-  <si>
-    <t>Efetivada</t>
-  </si>
-  <si>
     <t>Rejeitada para Resolução</t>
   </si>
   <si>
@@ -78,6 +72,9 @@
   </si>
   <si>
     <t>SAR03</t>
+  </si>
+  <si>
+    <t>Efetivada e Encerrada</t>
   </si>
 </sst>
 </file>
@@ -460,13 +457,13 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" customWidth="1"/>
     <col min="6" max="6" width="23" customWidth="1"/>
@@ -486,70 +483,70 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E2" s="5">
         <v>42144</v>
       </c>
       <c r="F2" s="5">
-        <v>42144</v>
+        <v>42145</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E3" s="5">
         <v>42144</v>
       </c>
       <c r="F3" s="5">
-        <v>42144</v>
+        <v>42145</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E4" s="5">
         <v>42144</v>
       </c>
       <c r="F4" s="5">
-        <v>42144</v>
+        <v>42145</v>
       </c>
     </row>
   </sheetData>
@@ -564,10 +561,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,10 +590,10 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -607,16 +604,16 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -624,7 +621,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -632,17 +629,12 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Efetivando as SARs aprovadas no EVE-EOR.
</commit_message>
<xml_diff>
--- a/Artefatos de Documentação/Processo Aplicado/EveRemind/1-Gerencia de Requisitos/Histórico de SARs.xlsx
+++ b/Artefatos de Documentação/Processo Aplicado/EveRemind/1-Gerencia de Requisitos/Histórico de SARs.xlsx
@@ -74,7 +74,7 @@
     <t>SAR03</t>
   </si>
   <si>
-    <t>Efetivada e Encerrada</t>
+    <t>Efetivada no EOR</t>
   </si>
 </sst>
 </file>
@@ -457,7 +457,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,7 +497,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>15</v>
@@ -517,7 +517,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>15</v>
@@ -537,7 +537,7 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>15</v>
@@ -564,7 +564,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>